<commit_message>
Both attacks for AI
</commit_message>
<xml_diff>
--- a/Assets/GameDocument.xlsx
+++ b/Assets/GameDocument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Victor\Proyectos\Repositories\CombatAI\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4A7489-627C-4AA3-8255-CF43D3206A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4437BC39-50A9-45F9-A075-734476E27D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3084" yWindow="0" windowWidth="21600" windowHeight="11328" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Animation List</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Timmed attacks / combos</t>
+  </si>
+  <si>
+    <t>Allow character to sligly move during attack animations</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
   <dimension ref="B2:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +588,9 @@
       </c>
     </row>
     <row r="8" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>

</xml_diff>